<commit_message>
Update function for general function
</commit_message>
<xml_diff>
--- a/Testcase/Automation_Call cheat.xlsx
+++ b/Testcase/Automation_Call cheat.xlsx
@@ -5,16 +5,16 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db211ccea624a480/Documents/GitHub/Evn-Automation-tool/Testcase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nexono365-my.sharepoint.com/personal/evan_nexonnetworks_com/Documents/[Demostration] V4 Gacha test/Testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="215" documentId="13_ncr:1_{041359F6-5613-46A6-A6D4-115A2ABAF22A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ECD9C29D-F91F-46DE-9FC1-60ABE6872E94}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="13_ncr:1_{041359F6-5613-46A6-A6D4-115A2ABAF22A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3BDA2680-9DD2-4DF4-9DF4-C47636DDC0D0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="826" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" tabRatio="826" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Result" sheetId="49" r:id="rId1"/>
-    <sheet name="Testcase" sheetId="44" r:id="rId2"/>
+    <sheet name="Testcase" sheetId="44" r:id="rId1"/>
+    <sheet name="Result" sheetId="49" r:id="rId2"/>
     <sheet name="Data_CheatList" sheetId="48" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="37">
   <si>
     <t>StringID</t>
   </si>
@@ -147,12 +147,6 @@
   </si>
   <si>
     <t>Number of item on screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//type of script --&gt; for tool to prepare necessary lib </t>
-  </si>
-  <si>
-    <t>//type of Gacha need test --&gt; need prepare the needed sheet in DB file, link with DB file</t>
   </si>
   <si>
     <t>//list function will be provided later</t>
@@ -201,7 +195,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -252,6 +246,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Malgun Gothic"/>
       <family val="2"/>
     </font>
@@ -355,7 +356,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -404,6 +405,9 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -411,7 +415,7 @@
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="36">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -424,6 +428,66 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -699,96 +763,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1111,6 +1085,364 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8D73BA-C301-47A9-B5A2-51E4ECFCF070}">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="25.625" customWidth="1"/>
+    <col min="3" max="8" width="30.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="13"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B1:B11 B21:B1048576">
+    <cfRule type="containsText" dxfId="35" priority="256" operator="containsText" text="Loop">
+      <formula>NOT(ISERROR(SEARCH("Loop",B1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="257" operator="equal">
+      <formula>"Result"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="260" operator="equal">
+      <formula>"Step"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="containsText" dxfId="32" priority="163" operator="containsText" text="Loop">
+      <formula>NOT(ISERROR(SEARCH("Loop",B13)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="164" operator="equal">
+      <formula>"Result"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="165" operator="equal">
+      <formula>"Step"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="containsText" dxfId="29" priority="136" operator="containsText" text="Loop">
+      <formula>NOT(ISERROR(SEARCH("Loop",B16)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="137" operator="equal">
+      <formula>"Result"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="138" operator="equal">
+      <formula>"Step"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="containsText" dxfId="26" priority="133" operator="containsText" text="Loop">
+      <formula>NOT(ISERROR(SEARCH("Loop",B17)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="134" operator="equal">
+      <formula>"Result"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="135" operator="equal">
+      <formula>"Step"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="containsText" dxfId="23" priority="166" operator="containsText" text="Loop">
+      <formula>NOT(ISERROR(SEARCH("Loop",B12)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="167" operator="equal">
+      <formula>"Result"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="168" operator="equal">
+      <formula>"Step"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="containsText" dxfId="20" priority="103" operator="containsText" text="Loop">
+      <formula>NOT(ISERROR(SEARCH("Loop",B18)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="104" operator="equal">
+      <formula>"Result"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="105" operator="equal">
+      <formula>"Step"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="containsText" dxfId="17" priority="100" operator="containsText" text="Loop">
+      <formula>NOT(ISERROR(SEARCH("Loop",B19)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="101" operator="equal">
+      <formula>"Result"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="102" operator="equal">
+      <formula>"Step"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="containsText" dxfId="14" priority="43" operator="containsText" text="Loop">
+      <formula>NOT(ISERROR(SEARCH("Loop",B14)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="44" operator="equal">
+      <formula>"Result"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="45" operator="equal">
+      <formula>"Step"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="containsText" dxfId="11" priority="37" operator="containsText" text="Loop">
+      <formula>NOT(ISERROR(SEARCH("Loop",B15)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="38" operator="equal">
+      <formula>"Result"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="39" operator="equal">
+      <formula>"Step"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Loop">
+      <formula>NOT(ISERROR(SEARCH("Loop",B20)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"Result"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>"Step"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFEE3D2A-8366-471E-87D4-7C399924C771}">
   <dimension ref="A10:D50"/>
   <sheetViews>
@@ -1461,394 +1793,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
-    <cfRule type="cellIs" dxfId="38" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"Loop"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"Step"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Loop"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Step"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Loop"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Step"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8D73BA-C301-47A9-B5A2-51E4ECFCF070}">
-  <dimension ref="A1:H20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="25.625" customWidth="1"/>
-    <col min="3" max="8" width="30.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C10" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B1:B11 B21:B1048576">
-    <cfRule type="containsText" dxfId="32" priority="256" operator="containsText" text="Loop">
-      <formula>NOT(ISERROR(SEARCH("Loop",B1)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="257" operator="equal">
-      <formula>"Result"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="260" operator="equal">
-      <formula>"Step"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
-    <cfRule type="containsText" dxfId="29" priority="163" operator="containsText" text="Loop">
-      <formula>NOT(ISERROR(SEARCH("Loop",B13)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="164" operator="equal">
-      <formula>"Result"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="165" operator="equal">
-      <formula>"Step"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="26" priority="136" operator="containsText" text="Loop">
-      <formula>NOT(ISERROR(SEARCH("Loop",B16)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="137" operator="equal">
-      <formula>"Result"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="138" operator="equal">
-      <formula>"Step"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="containsText" dxfId="23" priority="133" operator="containsText" text="Loop">
-      <formula>NOT(ISERROR(SEARCH("Loop",B17)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="134" operator="equal">
-      <formula>"Result"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="135" operator="equal">
-      <formula>"Step"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
-    <cfRule type="containsText" dxfId="20" priority="166" operator="containsText" text="Loop">
-      <formula>NOT(ISERROR(SEARCH("Loop",B12)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="167" operator="equal">
-      <formula>"Result"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="168" operator="equal">
-      <formula>"Step"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="containsText" dxfId="17" priority="103" operator="containsText" text="Loop">
-      <formula>NOT(ISERROR(SEARCH("Loop",B18)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="104" operator="equal">
-      <formula>"Result"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="105" operator="equal">
-      <formula>"Step"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="14" priority="100" operator="containsText" text="Loop">
-      <formula>NOT(ISERROR(SEARCH("Loop",B19)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="101" operator="equal">
-      <formula>"Result"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="102" operator="equal">
-      <formula>"Step"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="11" priority="43" operator="containsText" text="Loop">
-      <formula>NOT(ISERROR(SEARCH("Loop",B14)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="44" operator="equal">
-      <formula>"Result"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="45" operator="equal">
-      <formula>"Step"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="8" priority="37" operator="containsText" text="Loop">
-      <formula>NOT(ISERROR(SEARCH("Loop",B15)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="38" operator="equal">
-      <formula>"Result"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="39" operator="equal">
-      <formula>"Step"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Loop">
-      <formula>NOT(ISERROR(SEARCH("Loop",B20)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
-      <formula>"Result"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
-      <formula>"Step"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1856,13 +1824,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F5E3D1-7736-411C-ADA8-FAD22A761938}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1872,26 +1841,26 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>